<commit_message>
dictionary, codelist and etl output up to poverty
</commit_message>
<xml_diff>
--- a/tmee/data_in/data_dictionary/indicator_dictionary_TM_v8.xlsx
+++ b/tmee/data_in/data_dictionary/indicator_dictionary_TM_v8.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/16f1c7c3db740efb/UNICEF/TransMonEE/data-etl/tmee/data_in/data_dictionary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1038" documentId="8_{C78D5DBA-9509-40B0-B726-8EC80EC5AE84}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{FDA6DCE4-73B5-4EFC-BB3B-6C92FF3A9B47}"/>
+  <xr:revisionPtr revIDLastSave="1058" documentId="8_{C78D5DBA-9509-40B0-B726-8EC80EC5AE84}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{319250F9-916A-463E-9AF0-737BE134983E}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8993" uniqueCount="4218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9002" uniqueCount="4220">
   <si>
     <t>snapshot_id</t>
   </si>
@@ -12698,6 +12698,12 @@
   </si>
   <si>
     <t>Percentage (by sex, age groups and wealth quintile)</t>
+  </si>
+  <si>
+    <t>Not reporting data for ECARO as of 07/07/2021</t>
+  </si>
+  <si>
+    <t>Indicator without data for the region as of 07/07/2021</t>
   </si>
 </sst>
 </file>
@@ -13497,7 +13503,7 @@
   <dimension ref="A1:L386"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A299" workbookViewId="0">
-      <selection activeCell="F316" sqref="F316:G316"/>
+      <selection activeCell="G309" sqref="G309"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -23949,8 +23955,13 @@
       <c r="E307" s="1">
         <v>2021</v>
       </c>
-      <c r="F307" s="1"/>
-      <c r="G307" s="1"/>
+      <c r="F307" s="1" t="s">
+        <v>2470</v>
+      </c>
+      <c r="G307" s="1" t="str">
+        <f>VLOOKUP(F307,Value_type!$A$2:$I$107,3,FALSE)</f>
+        <v>-</v>
+      </c>
       <c r="H307" s="1" t="s">
         <v>3516</v>
       </c>
@@ -23978,8 +23989,13 @@
       <c r="E308" s="1">
         <v>2021</v>
       </c>
-      <c r="F308" s="1"/>
-      <c r="G308" s="1"/>
+      <c r="F308" s="1" t="s">
+        <v>2470</v>
+      </c>
+      <c r="G308" s="1" t="str">
+        <f>VLOOKUP(F308,Value_type!$A$2:$I$107,3,FALSE)</f>
+        <v>-</v>
+      </c>
       <c r="H308" s="1" t="s">
         <v>3517</v>
       </c>
@@ -27145,8 +27161,8 @@
   <dimension ref="A1:M832"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A355" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E370" sqref="E370"/>
+      <pane ySplit="1" topLeftCell="A358" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M362" sqref="M362"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -34605,7 +34621,7 @@
       <c r="I352"/>
       <c r="J352"/>
     </row>
-    <row r="353" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="353" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A353" s="16" t="s">
         <v>1472</v>
       </c>
@@ -34627,7 +34643,7 @@
       <c r="I353"/>
       <c r="J353"/>
     </row>
-    <row r="354" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="354" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A354" s="16" t="s">
         <v>1474</v>
       </c>
@@ -34649,7 +34665,7 @@
       <c r="I354"/>
       <c r="J354"/>
     </row>
-    <row r="355" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="355" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A355" s="16" t="s">
         <v>1476</v>
       </c>
@@ -34671,7 +34687,7 @@
       <c r="I355"/>
       <c r="J355"/>
     </row>
-    <row r="356" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="356" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A356" s="16" t="s">
         <v>1478</v>
       </c>
@@ -34693,7 +34709,7 @@
       <c r="I356"/>
       <c r="J356"/>
     </row>
-    <row r="357" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="357" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A357" s="16" t="s">
         <v>1480</v>
       </c>
@@ -34715,7 +34731,7 @@
       <c r="I357"/>
       <c r="J357"/>
     </row>
-    <row r="358" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="358" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A358" s="16" t="s">
         <v>1482</v>
       </c>
@@ -34737,7 +34753,7 @@
       <c r="I358"/>
       <c r="J358"/>
     </row>
-    <row r="359" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="359" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A359" s="16" t="s">
         <v>1484</v>
       </c>
@@ -34759,7 +34775,7 @@
       <c r="I359"/>
       <c r="J359"/>
     </row>
-    <row r="360" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="360" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A360" s="16" t="s">
         <v>1486</v>
       </c>
@@ -34781,7 +34797,7 @@
       <c r="I360"/>
       <c r="J360"/>
     </row>
-    <row r="361" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="361" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A361" s="16" t="s">
         <v>1488</v>
       </c>
@@ -34802,8 +34818,11 @@
       </c>
       <c r="I361"/>
       <c r="J361"/>
-    </row>
-    <row r="362" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="M361" s="37" t="s">
+        <v>4218</v>
+      </c>
+    </row>
+    <row r="362" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A362" s="16" t="s">
         <v>1490</v>
       </c>
@@ -34824,8 +34843,11 @@
       </c>
       <c r="I362"/>
       <c r="J362"/>
-    </row>
-    <row r="363" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="M362" s="37" t="s">
+        <v>4218</v>
+      </c>
+    </row>
+    <row r="363" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A363" s="16" t="s">
         <v>1492</v>
       </c>
@@ -34847,7 +34869,7 @@
       <c r="I363"/>
       <c r="J363"/>
     </row>
-    <row r="364" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="364" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A364" s="16" t="s">
         <v>1494</v>
       </c>
@@ -34869,7 +34891,7 @@
       <c r="I364"/>
       <c r="J364"/>
     </row>
-    <row r="365" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="365" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A365" s="16" t="s">
         <v>1496</v>
       </c>
@@ -34891,7 +34913,7 @@
       <c r="I365"/>
       <c r="J365"/>
     </row>
-    <row r="366" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="366" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A366" s="16" t="s">
         <v>1498</v>
       </c>
@@ -34913,7 +34935,7 @@
       <c r="I366"/>
       <c r="J366"/>
     </row>
-    <row r="367" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="367" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A367" s="16" t="s">
         <v>1500</v>
       </c>
@@ -34935,7 +34957,7 @@
       <c r="I367"/>
       <c r="J367"/>
     </row>
-    <row r="368" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="368" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A368" s="16" t="s">
         <v>1501</v>
       </c>
@@ -40847,8 +40869,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:L107"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="H32" sqref="H32"/>
+    <sheetView topLeftCell="A94" workbookViewId="0">
+      <selection activeCell="I108" sqref="I108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -42075,59 +42097,74 @@
         <v>624</v>
       </c>
     </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A97" s="1" t="s">
         <v>625</v>
       </c>
     </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A98" s="1" t="s">
         <v>626</v>
       </c>
     </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A99" s="1" t="s">
         <v>627</v>
       </c>
     </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A100" s="1" t="s">
         <v>628</v>
       </c>
     </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A101" s="1" t="s">
         <v>2464</v>
       </c>
     </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A102" s="1" t="s">
         <v>2465</v>
       </c>
     </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A103" s="1" t="s">
         <v>2466</v>
       </c>
     </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A104" s="1" t="s">
         <v>2467</v>
       </c>
     </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A105" s="1" t="s">
         <v>2468</v>
       </c>
     </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A106" s="1" t="s">
         <v>2469</v>
       </c>
     </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A107" s="1" t="s">
         <v>2470</v>
+      </c>
+      <c r="B107" s="1" t="s">
+        <v>536</v>
+      </c>
+      <c r="C107" s="1" t="s">
+        <v>2019</v>
+      </c>
+      <c r="G107" s="1" t="s">
+        <v>2019</v>
+      </c>
+      <c r="H107" s="25" t="s">
+        <v>2019</v>
+      </c>
+      <c r="I107" t="s">
+        <v>4219</v>
       </c>
     </row>
   </sheetData>
@@ -42141,7 +42178,7 @@
   <dimension ref="A1:K394"/>
   <sheetViews>
     <sheetView topLeftCell="A304" workbookViewId="0">
-      <selection activeCell="D318" sqref="D318"/>
+      <selection activeCell="I313" sqref="I313"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
child rights addition to DB
</commit_message>
<xml_diff>
--- a/tmee/data_in/data_dictionary/indicator_dictionary_TM_v8.xlsx
+++ b/tmee/data_in/data_dictionary/indicator_dictionary_TM_v8.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/16f1c7c3db740efb/UNICEF/TransMonEE/data-etl/tmee/data_in/data_dictionary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="353" documentId="13_ncr:1_{D6446E56-D0B6-414D-A4F6-23CFDA12394E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{7A7D36D9-FFFC-4194-BEEE-A9CD8C3BC347}"/>
+  <xr:revisionPtr revIDLastSave="364" documentId="13_ncr:1_{D6446E56-D0B6-414D-A4F6-23CFDA12394E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{F08FC8EA-0E32-4728-8D9A-5C1DD316BCAC}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9473" uniqueCount="4409">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9473" uniqueCount="4418">
   <si>
     <t>snapshot_id</t>
   </si>
@@ -13271,6 +13271,33 @@
   </si>
   <si>
     <t>US$</t>
+  </si>
+  <si>
+    <t>SDG: SG_STT_NSDSFND</t>
+  </si>
+  <si>
+    <t>SDG: SG_STT_NSDSIMPL</t>
+  </si>
+  <si>
+    <t>SDG: SG_STT_NSDSFDGVT</t>
+  </si>
+  <si>
+    <t>SDG: SG_STT_NSDSFDDNR</t>
+  </si>
+  <si>
+    <t>SDG: SG_STT_NSDSFDOTHR</t>
+  </si>
+  <si>
+    <t>SDG: SG_STT_CAPTY</t>
+  </si>
+  <si>
+    <t>SDG: SG_REG_CENSUSN</t>
+  </si>
+  <si>
+    <t>SDG: SG_REG_BRTH90N</t>
+  </si>
+  <si>
+    <t>SDG: SG_REG_DETH75N</t>
   </si>
 </sst>
 </file>
@@ -14069,7 +14096,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L411"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A364" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A361" workbookViewId="0">
       <selection activeCell="F376" sqref="F376:G376"/>
     </sheetView>
   </sheetViews>
@@ -26608,7 +26635,7 @@
       </c>
       <c r="I368" s="25" t="str">
         <f>VLOOKUP(H368,Source!$A$2:$G$452,3,FALSE)</f>
-        <v>CR_SG_STT_NSDSFND</v>
+        <v>SDG: SG_STT_NSDSFND</v>
       </c>
       <c r="K368" s="1"/>
     </row>
@@ -26642,7 +26669,7 @@
       </c>
       <c r="I369" s="25" t="str">
         <f>VLOOKUP(H369,Source!$A$2:$G$452,3,FALSE)</f>
-        <v>CR_SG_STT_NSDSIMPL</v>
+        <v>SDG: SG_STT_NSDSIMPL</v>
       </c>
       <c r="K369" s="1"/>
     </row>
@@ -26676,7 +26703,7 @@
       </c>
       <c r="I370" s="25" t="str">
         <f>VLOOKUP(H370,Source!$A$2:$G$452,3,FALSE)</f>
-        <v>CR_SG_STT_NSDSFDGVT</v>
+        <v>SDG: SG_STT_NSDSFDGVT</v>
       </c>
       <c r="K370" s="1"/>
     </row>
@@ -26710,7 +26737,7 @@
       </c>
       <c r="I371" s="25" t="str">
         <f>VLOOKUP(H371,Source!$A$2:$G$452,3,FALSE)</f>
-        <v>CR_SG_STT_NSDSFDDNR</v>
+        <v>SDG: SG_STT_NSDSFDDNR</v>
       </c>
       <c r="K371" s="1"/>
     </row>
@@ -26744,7 +26771,7 @@
       </c>
       <c r="I372" s="25" t="str">
         <f>VLOOKUP(H372,Source!$A$2:$G$452,3,FALSE)</f>
-        <v>CR_SG_STT_NSDSFDOTHR</v>
+        <v>SDG: SG_STT_NSDSFDOTHR</v>
       </c>
       <c r="K372" s="1"/>
     </row>
@@ -26778,7 +26805,7 @@
       </c>
       <c r="I373" s="25" t="str">
         <f>VLOOKUP(H373,Source!$A$2:$G$452,3,FALSE)</f>
-        <v>CR_SG_STT_CAPTY</v>
+        <v>SDG: SG_STT_CAPTY</v>
       </c>
       <c r="K373" s="1"/>
     </row>
@@ -26812,7 +26839,7 @@
       </c>
       <c r="I374" s="25" t="str">
         <f>VLOOKUP(H374,Source!$A$2:$G$452,3,FALSE)</f>
-        <v>CR_SG_REG_CENSUSN</v>
+        <v>SDG: SG_REG_CENSUSN</v>
       </c>
       <c r="K374" s="1"/>
     </row>
@@ -26846,7 +26873,7 @@
       </c>
       <c r="I375" s="25" t="str">
         <f>VLOOKUP(H375,Source!$A$2:$G$452,3,FALSE)</f>
-        <v>CR_SG_REG_BRTH90N</v>
+        <v>SDG: SG_REG_BRTH90N</v>
       </c>
       <c r="K375" s="1"/>
     </row>
@@ -26880,7 +26907,7 @@
       </c>
       <c r="I376" s="25" t="str">
         <f>VLOOKUP(H376,Source!$A$2:$G$452,3,FALSE)</f>
-        <v>CR_SG_REG_DETH75N</v>
+        <v>SDG: SG_REG_DETH75N</v>
       </c>
       <c r="K376" s="1"/>
     </row>
@@ -44200,7 +44227,7 @@
   <dimension ref="A1:K419"/>
   <sheetViews>
     <sheetView topLeftCell="A364" workbookViewId="0">
-      <selection activeCell="E358" sqref="E358"/>
+      <selection activeCell="D382" sqref="D382"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -55015,7 +55042,7 @@
         <v>639</v>
       </c>
       <c r="C374" s="60" t="s">
-        <v>4266</v>
+        <v>4409</v>
       </c>
       <c r="D374" s="24" t="s">
         <v>4286</v>
@@ -55044,7 +55071,7 @@
         <v>639</v>
       </c>
       <c r="C375" s="60" t="s">
-        <v>4268</v>
+        <v>4410</v>
       </c>
       <c r="D375" s="24" t="s">
         <v>4288</v>
@@ -55073,7 +55100,7 @@
         <v>639</v>
       </c>
       <c r="C376" s="60" t="s">
-        <v>4270</v>
+        <v>4411</v>
       </c>
       <c r="D376" s="24" t="s">
         <v>4401</v>
@@ -55102,7 +55129,7 @@
         <v>639</v>
       </c>
       <c r="C377" s="60" t="s">
-        <v>4272</v>
+        <v>4412</v>
       </c>
       <c r="D377" s="24" t="s">
         <v>4289</v>
@@ -55131,7 +55158,7 @@
         <v>639</v>
       </c>
       <c r="C378" s="60" t="s">
-        <v>4274</v>
+        <v>4413</v>
       </c>
       <c r="D378" s="24" t="s">
         <v>4402</v>
@@ -55160,7 +55187,7 @@
         <v>639</v>
       </c>
       <c r="C379" s="60" t="s">
-        <v>4275</v>
+        <v>4414</v>
       </c>
       <c r="D379" s="24" t="s">
         <v>4291</v>
@@ -55189,7 +55216,7 @@
         <v>639</v>
       </c>
       <c r="C380" s="60" t="s">
-        <v>4278</v>
+        <v>4415</v>
       </c>
       <c r="D380" s="24" t="s">
         <v>4403</v>
@@ -55218,7 +55245,7 @@
         <v>639</v>
       </c>
       <c r="C381" s="60" t="s">
-        <v>4280</v>
+        <v>4416</v>
       </c>
       <c r="D381" s="24" t="s">
         <v>4292</v>
@@ -55247,7 +55274,7 @@
         <v>639</v>
       </c>
       <c r="C382" s="60" t="s">
-        <v>4282</v>
+        <v>4417</v>
       </c>
       <c r="D382" s="24" t="s">
         <v>4293</v>

</xml_diff>

<commit_message>
education repeaters not in dashboard added to subtopic
</commit_message>
<xml_diff>
--- a/tmee/data_in/data_dictionary/indicator_dictionary_TM_v8.xlsx
+++ b/tmee/data_in/data_dictionary/indicator_dictionary_TM_v8.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/16f1c7c3db740efb/UNICEF/TransMonEE/data-etl/tmee/data_in/data_dictionary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="30" documentId="13_ncr:1_{F4B63CBD-989C-41F1-BE67-2BCF2EE5BF3B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{25BB6BCF-EE86-4738-8B63-53D99134E498}"/>
+  <xr:revisionPtr revIDLastSave="33" documentId="13_ncr:1_{F4B63CBD-989C-41F1-BE67-2BCF2EE5BF3B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00D7D6B9-BD7C-4ED6-B594-AF0930FC54DA}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="19440" windowHeight="10440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29653,8 +29653,8 @@
   <dimension ref="A1:M877"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A283" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E298" sqref="E298"/>
+      <pane ySplit="1" topLeftCell="A232" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D240" sqref="D240"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -34681,7 +34681,7 @@
         <v>2317</v>
       </c>
       <c r="D237" s="25" t="s">
-        <v>2509</v>
+        <v>4272</v>
       </c>
       <c r="E237" s="50" t="s">
         <v>4357</v>
@@ -34701,7 +34701,7 @@
         <v>2317</v>
       </c>
       <c r="D238" s="25" t="s">
-        <v>2509</v>
+        <v>4272</v>
       </c>
       <c r="E238" s="50" t="s">
         <v>4358</v>
@@ -34721,7 +34721,7 @@
         <v>2317</v>
       </c>
       <c r="D239" s="25" t="s">
-        <v>2509</v>
+        <v>4272</v>
       </c>
       <c r="E239" s="50" t="s">
         <v>2510</v>

</xml_diff>

<commit_message>
binary units updated for selected indicators
</commit_message>
<xml_diff>
--- a/tmee/data_in/data_dictionary/indicator_dictionary_TM_v8.xlsx
+++ b/tmee/data_in/data_dictionary/indicator_dictionary_TM_v8.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/16f1c7c3db740efb/UNICEF/TransMonEE/data-etl/tmee/data_in/data_dictionary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="33" documentId="13_ncr:1_{F4B63CBD-989C-41F1-BE67-2BCF2EE5BF3B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00D7D6B9-BD7C-4ED6-B594-AF0930FC54DA}"/>
+  <xr:revisionPtr revIDLastSave="49" documentId="13_ncr:1_{F4B63CBD-989C-41F1-BE67-2BCF2EE5BF3B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{D33B7E5F-A0D0-4761-A7A4-B924DE6025B6}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="19440" windowHeight="10440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="19440" windowHeight="10440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Snapshot" sheetId="1" r:id="rId1"/>
@@ -14502,8 +14502,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L430"/>
   <sheetViews>
-    <sheetView topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="D98" sqref="D98"/>
+    <sheetView tabSelected="1" topLeftCell="A255" workbookViewId="0">
+      <selection activeCell="G269" sqref="G269"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -20536,11 +20536,11 @@
         <v>2020</v>
       </c>
       <c r="F177" s="1" t="s">
-        <v>551</v>
+        <v>561</v>
       </c>
       <c r="G177" s="1" t="str">
         <f>VLOOKUP(F177,Value_type!$A$2:$I$107,3,FALSE)</f>
-        <v>NUMBER</v>
+        <v>BINARY</v>
       </c>
       <c r="H177" s="1" t="s">
         <v>2073</v>
@@ -20570,11 +20570,11 @@
         <v>2020</v>
       </c>
       <c r="F178" s="1" t="s">
-        <v>551</v>
+        <v>561</v>
       </c>
       <c r="G178" s="1" t="str">
         <f>VLOOKUP(F178,Value_type!$A$2:$I$107,3,FALSE)</f>
-        <v>NUMBER</v>
+        <v>BINARY</v>
       </c>
       <c r="H178" s="1" t="s">
         <v>2074</v>
@@ -20604,11 +20604,11 @@
         <v>2020</v>
       </c>
       <c r="F179" s="1" t="s">
-        <v>551</v>
+        <v>561</v>
       </c>
       <c r="G179" s="1" t="str">
         <f>VLOOKUP(F179,Value_type!$A$2:$I$107,3,FALSE)</f>
-        <v>NUMBER</v>
+        <v>BINARY</v>
       </c>
       <c r="H179" s="1" t="s">
         <v>2075</v>
@@ -20638,11 +20638,11 @@
         <v>2020</v>
       </c>
       <c r="F180" s="1" t="s">
-        <v>551</v>
+        <v>561</v>
       </c>
       <c r="G180" s="1" t="str">
         <f>VLOOKUP(F180,Value_type!$A$2:$I$107,3,FALSE)</f>
-        <v>NUMBER</v>
+        <v>BINARY</v>
       </c>
       <c r="H180" s="1" t="s">
         <v>2076</v>
@@ -23630,11 +23630,11 @@
         <v>2020</v>
       </c>
       <c r="F268" s="1" t="s">
-        <v>551</v>
+        <v>561</v>
       </c>
       <c r="G268" s="1" t="str">
         <f>VLOOKUP(F268,Value_type!$A$2:$I$107,3,FALSE)</f>
-        <v>NUMBER</v>
+        <v>BINARY</v>
       </c>
       <c r="H268" s="1" t="s">
         <v>3030</v>
@@ -23664,11 +23664,11 @@
         <v>2020</v>
       </c>
       <c r="F269" s="1" t="s">
-        <v>551</v>
+        <v>561</v>
       </c>
       <c r="G269" s="1" t="str">
         <f>VLOOKUP(F269,Value_type!$A$2:$I$107,3,FALSE)</f>
-        <v>NUMBER</v>
+        <v>BINARY</v>
       </c>
       <c r="H269" s="1" t="s">
         <v>3031</v>
@@ -27116,11 +27116,11 @@
         <v>2021</v>
       </c>
       <c r="F370" s="1" t="s">
-        <v>551</v>
+        <v>561</v>
       </c>
       <c r="G370" s="1" t="str">
         <f>VLOOKUP(F370,Value_type!$A$2:$I$107,3,FALSE)</f>
-        <v>NUMBER</v>
+        <v>BINARY</v>
       </c>
       <c r="H370" s="1" t="s">
         <v>3798</v>
@@ -27150,11 +27150,11 @@
         <v>2021</v>
       </c>
       <c r="F371" s="1" t="s">
-        <v>551</v>
+        <v>561</v>
       </c>
       <c r="G371" s="1" t="str">
         <f>VLOOKUP(F371,Value_type!$A$2:$I$107,3,FALSE)</f>
-        <v>NUMBER</v>
+        <v>BINARY</v>
       </c>
       <c r="H371" s="1" t="s">
         <v>3856</v>
@@ -27184,11 +27184,11 @@
         <v>2021</v>
       </c>
       <c r="F372" s="1" t="s">
-        <v>551</v>
+        <v>561</v>
       </c>
       <c r="G372" s="1" t="str">
         <f>VLOOKUP(F372,Value_type!$A$2:$I$107,3,FALSE)</f>
-        <v>NUMBER</v>
+        <v>BINARY</v>
       </c>
       <c r="H372" s="1" t="s">
         <v>3857</v>
@@ -27218,11 +27218,11 @@
         <v>2021</v>
       </c>
       <c r="F373" s="1" t="s">
-        <v>551</v>
+        <v>561</v>
       </c>
       <c r="G373" s="1" t="str">
         <f>VLOOKUP(F373,Value_type!$A$2:$I$107,3,FALSE)</f>
-        <v>NUMBER</v>
+        <v>BINARY</v>
       </c>
       <c r="H373" s="1" t="s">
         <v>3858</v>
@@ -27252,11 +27252,11 @@
         <v>2021</v>
       </c>
       <c r="F374" s="1" t="s">
-        <v>551</v>
+        <v>561</v>
       </c>
       <c r="G374" s="1" t="str">
         <f>VLOOKUP(F374,Value_type!$A$2:$I$107,3,FALSE)</f>
-        <v>NUMBER</v>
+        <v>BINARY</v>
       </c>
       <c r="H374" s="1" t="s">
         <v>3859</v>
@@ -27286,11 +27286,11 @@
         <v>2021</v>
       </c>
       <c r="F375" s="1" t="s">
-        <v>551</v>
+        <v>561</v>
       </c>
       <c r="G375" s="1" t="str">
         <f>VLOOKUP(F375,Value_type!$A$2:$I$107,3,FALSE)</f>
-        <v>NUMBER</v>
+        <v>BINARY</v>
       </c>
       <c r="H375" s="1" t="s">
         <v>3860</v>
@@ -27354,11 +27354,11 @@
         <v>2021</v>
       </c>
       <c r="F377" s="1" t="s">
-        <v>551</v>
+        <v>561</v>
       </c>
       <c r="G377" s="1" t="str">
         <f>VLOOKUP(F377,Value_type!$A$2:$I$107,3,FALSE)</f>
-        <v>NUMBER</v>
+        <v>BINARY</v>
       </c>
       <c r="H377" s="1" t="s">
         <v>3917</v>
@@ -27939,11 +27939,11 @@
         <v>PCNT</v>
       </c>
       <c r="H394" s="1" t="s">
-        <v>4073</v>
+        <v>4076</v>
       </c>
       <c r="I394" s="25" t="str">
         <f>VLOOKUP(H394,Source!$A$2:$G$471,3,FALSE)</f>
-        <v>Helix: PT_F_15-49_W-BTNG</v>
+        <v>Helix: PT_F_15-19_MRD</v>
       </c>
       <c r="K394" s="1"/>
     </row>
@@ -27973,11 +27973,11 @@
         <v>PCNT</v>
       </c>
       <c r="H395" s="1" t="s">
-        <v>4074</v>
+        <v>4077</v>
       </c>
       <c r="I395" s="25" t="str">
         <f>VLOOKUP(H395,Source!$A$2:$G$471,3,FALSE)</f>
-        <v>Helix: PT_M_15-49_W-BTNG</v>
+        <v>Helix: PT_M_15-19_MRD</v>
       </c>
       <c r="K395" s="1"/>
     </row>
@@ -28007,11 +28007,11 @@
         <v>PCNT</v>
       </c>
       <c r="H396" s="1" t="s">
-        <v>4075</v>
+        <v>4078</v>
       </c>
       <c r="I396" s="25" t="str">
         <f>VLOOKUP(H396,Source!$A$2:$G$471,3,FALSE)</f>
-        <v>Helix: PT_ST_13-15_BUL_30-DYS</v>
+        <v>Helix: PT_F_20-24_MRD_U15</v>
       </c>
       <c r="K396" s="1"/>
     </row>
@@ -28041,11 +28041,11 @@
         <v>PCNT</v>
       </c>
       <c r="H397" s="1" t="s">
-        <v>4076</v>
+        <v>4079</v>
       </c>
       <c r="I397" s="25" t="str">
         <f>VLOOKUP(H397,Source!$A$2:$G$471,3,FALSE)</f>
-        <v>Helix: PT_F_15-19_MRD</v>
+        <v>Helix: PT_F_20-24_MRD_U18</v>
       </c>
       <c r="K397" s="1"/>
     </row>
@@ -28075,11 +28075,11 @@
         <v>PCNT</v>
       </c>
       <c r="H398" s="1" t="s">
-        <v>4077</v>
+        <v>4080</v>
       </c>
       <c r="I398" s="25" t="str">
         <f>VLOOKUP(H398,Source!$A$2:$G$471,3,FALSE)</f>
-        <v>Helix: PT_M_15-19_MRD</v>
+        <v>Helix: PT_M_20-24_MRD_U18</v>
       </c>
       <c r="K398" s="1"/>
     </row>
@@ -28109,11 +28109,11 @@
         <v>PCNT</v>
       </c>
       <c r="H399" s="1" t="s">
-        <v>4078</v>
+        <v>4081</v>
       </c>
       <c r="I399" s="25" t="str">
         <f>VLOOKUP(H399,Source!$A$2:$G$471,3,FALSE)</f>
-        <v>Helix: PT_F_20-24_MRD_U15</v>
+        <v>Helix: PT_CHLD_5-17_LBR_ECON</v>
       </c>
       <c r="K399" s="1"/>
     </row>
@@ -28143,11 +28143,11 @@
         <v>PCNT</v>
       </c>
       <c r="H400" s="1" t="s">
-        <v>4079</v>
+        <v>4082</v>
       </c>
       <c r="I400" s="25" t="str">
         <f>VLOOKUP(H400,Source!$A$2:$G$471,3,FALSE)</f>
-        <v>Helix: PT_F_20-24_MRD_U18</v>
+        <v>Helix: PT_CHLD_5-17_LBR_ECON-HC</v>
       </c>
       <c r="K400" s="1"/>
     </row>
@@ -28177,11 +28177,11 @@
         <v>PCNT</v>
       </c>
       <c r="H401" s="1" t="s">
-        <v>4080</v>
+        <v>4083</v>
       </c>
       <c r="I401" s="25" t="str">
         <f>VLOOKUP(H401,Source!$A$2:$G$471,3,FALSE)</f>
-        <v>Helix: PT_M_20-24_MRD_U18</v>
+        <v>SDG: VC_PRS_UNSNT</v>
       </c>
       <c r="K401" s="1"/>
     </row>
@@ -28211,11 +28211,11 @@
         <v>NUMBER</v>
       </c>
       <c r="H402" s="1" t="s">
-        <v>4081</v>
+        <v>4084</v>
       </c>
       <c r="I402" s="25" t="str">
         <f>VLOOKUP(H402,Source!$A$2:$G$471,3,FALSE)</f>
-        <v>Helix: PT_CHLD_5-17_LBR_ECON</v>
+        <v>ESTAT: JJ_PRISIONERS</v>
       </c>
       <c r="K402" s="1"/>
     </row>
@@ -28245,11 +28245,11 @@
         <v>RATE_100000</v>
       </c>
       <c r="H403" s="1" t="s">
-        <v>4082</v>
+        <v>4085</v>
       </c>
       <c r="I403" s="25" t="str">
         <f>VLOOKUP(H403,Source!$A$2:$G$471,3,FALSE)</f>
-        <v>Helix: PT_CHLD_5-17_LBR_ECON-HC</v>
+        <v>ESTAT: JJ_PRISIONERS_RT</v>
       </c>
     </row>
     <row r="404" spans="1:11" x14ac:dyDescent="0.35">
@@ -28278,11 +28278,11 @@
         <v>PCNT</v>
       </c>
       <c r="H404" s="1" t="s">
-        <v>4083</v>
+        <v>4086</v>
       </c>
       <c r="I404" s="25" t="str">
         <f>VLOOKUP(H404,Source!$A$2:$G$471,3,FALSE)</f>
-        <v>SDG: VC_PRS_UNSNT</v>
+        <v>Helix: PT_CHLD_Y0T4_REG</v>
       </c>
     </row>
     <row r="405" spans="1:11" x14ac:dyDescent="0.35">
@@ -28304,18 +28304,18 @@
         <v>2021</v>
       </c>
       <c r="F405" s="1" t="s">
-        <v>551</v>
+        <v>561</v>
       </c>
       <c r="G405" s="1" t="str">
         <f>VLOOKUP(F405,Value_type!$A$2:$I$107,3,FALSE)</f>
-        <v>NUMBER</v>
+        <v>BINARY</v>
       </c>
       <c r="H405" s="1" t="s">
-        <v>4084</v>
+        <v>4087</v>
       </c>
       <c r="I405" s="25" t="str">
         <f>VLOOKUP(H405,Source!$A$2:$G$471,3,FALSE)</f>
-        <v>ESTAT: JJ_PRISIONERS</v>
+        <v>SDG: SG_REG_BRTH90N</v>
       </c>
     </row>
     <row r="406" spans="1:11" x14ac:dyDescent="0.35">
@@ -28337,18 +28337,18 @@
         <v>2021</v>
       </c>
       <c r="F406" s="1" t="s">
-        <v>551</v>
+        <v>561</v>
       </c>
       <c r="G406" s="1" t="str">
         <f>VLOOKUP(F406,Value_type!$A$2:$I$107,3,FALSE)</f>
-        <v>NUMBER</v>
+        <v>BINARY</v>
       </c>
       <c r="H406" s="1" t="s">
-        <v>4085</v>
+        <v>4088</v>
       </c>
       <c r="I406" s="25" t="str">
         <f>VLOOKUP(H406,Source!$A$2:$G$471,3,FALSE)</f>
-        <v>ESTAT: JJ_PRISIONERS_RT</v>
+        <v>SDG: SG_REG_DETH75N</v>
       </c>
     </row>
     <row r="407" spans="1:11" x14ac:dyDescent="0.35">
@@ -28370,18 +28370,18 @@
         <v>2021</v>
       </c>
       <c r="F407" s="1" t="s">
-        <v>551</v>
+        <v>561</v>
       </c>
       <c r="G407" s="1" t="str">
         <f>VLOOKUP(F407,Value_type!$A$2:$I$107,3,FALSE)</f>
-        <v>NUMBER</v>
+        <v>BINARY</v>
       </c>
       <c r="H407" s="1" t="s">
-        <v>4086</v>
+        <v>4089</v>
       </c>
       <c r="I407" s="25" t="str">
         <f>VLOOKUP(H407,Source!$A$2:$G$471,3,FALSE)</f>
-        <v>Helix: PT_CHLD_Y0T4_REG</v>
+        <v>SDG: SG_NHR_IMPLN</v>
       </c>
     </row>
     <row r="408" spans="1:11" x14ac:dyDescent="0.35">
@@ -28403,18 +28403,18 @@
         <v>2021</v>
       </c>
       <c r="F408" s="1" t="s">
-        <v>551</v>
+        <v>561</v>
       </c>
       <c r="G408" s="1" t="str">
         <f>VLOOKUP(F408,Value_type!$A$2:$I$107,3,FALSE)</f>
-        <v>NUMBER</v>
+        <v>BINARY</v>
       </c>
       <c r="H408" s="1" t="s">
-        <v>4087</v>
+        <v>4090</v>
       </c>
       <c r="I408" s="25" t="str">
         <f>VLOOKUP(H408,Source!$A$2:$G$471,3,FALSE)</f>
-        <v>SDG: SG_REG_BRTH90N</v>
+        <v>SDG: SG_NHR_INTEXSTN</v>
       </c>
     </row>
     <row r="409" spans="1:11" x14ac:dyDescent="0.35">
@@ -28436,18 +28436,18 @@
         <v>2021</v>
       </c>
       <c r="F409" s="1" t="s">
-        <v>551</v>
+        <v>561</v>
       </c>
       <c r="G409" s="1" t="str">
         <f>VLOOKUP(F409,Value_type!$A$2:$I$107,3,FALSE)</f>
-        <v>NUMBER</v>
+        <v>BINARY</v>
       </c>
       <c r="H409" s="1" t="s">
-        <v>4088</v>
+        <v>4091</v>
       </c>
       <c r="I409" s="25" t="str">
         <f>VLOOKUP(H409,Source!$A$2:$G$471,3,FALSE)</f>
-        <v>SDG: SG_REG_DETH75N</v>
+        <v>SDG: SG_NHR_NOSTUSN</v>
       </c>
     </row>
     <row r="410" spans="1:11" x14ac:dyDescent="0.35">
@@ -28469,18 +28469,18 @@
         <v>2021</v>
       </c>
       <c r="F410" s="1" t="s">
-        <v>551</v>
+        <v>561</v>
       </c>
       <c r="G410" s="1" t="str">
         <f>VLOOKUP(F410,Value_type!$A$2:$I$107,3,FALSE)</f>
-        <v>NUMBER</v>
+        <v>BINARY</v>
       </c>
       <c r="H410" s="1" t="s">
-        <v>4089</v>
+        <v>4092</v>
       </c>
       <c r="I410" s="25" t="str">
         <f>VLOOKUP(H410,Source!$A$2:$G$471,3,FALSE)</f>
-        <v>SDG: SG_NHR_IMPLN</v>
+        <v>SDG: SG_NHR_NOAPPLN</v>
       </c>
     </row>
     <row r="411" spans="1:11" x14ac:dyDescent="0.35">
@@ -28509,11 +28509,11 @@
         <v>RATE_100</v>
       </c>
       <c r="H411" s="1" t="s">
-        <v>4090</v>
+        <v>4124</v>
       </c>
       <c r="I411" s="25" t="str">
         <f>VLOOKUP(H411,Source!$A$2:$G$471,3,FALSE)</f>
-        <v>SDG: SG_NHR_INTEXSTN</v>
+        <v>SDG: IT_USE_ii99</v>
       </c>
     </row>
     <row r="412" spans="1:11" x14ac:dyDescent="0.35">
@@ -28542,11 +28542,11 @@
         <v>PCNT</v>
       </c>
       <c r="H412" s="1" t="s">
-        <v>4091</v>
+        <v>4125</v>
       </c>
       <c r="I412" s="25" t="str">
         <f>VLOOKUP(H412,Source!$A$2:$G$471,3,FALSE)</f>
-        <v>SDG: SG_NHR_NOSTUSN</v>
+        <v>SDG: SE_ADT_ACTS</v>
       </c>
     </row>
     <row r="413" spans="1:11" x14ac:dyDescent="0.35">
@@ -28575,11 +28575,11 @@
         <v>PCNT</v>
       </c>
       <c r="H413" s="1" t="s">
-        <v>4092</v>
+        <v>4239</v>
       </c>
       <c r="I413" s="25" t="str">
         <f>VLOOKUP(H413,Source!$A$2:$G$471,3,FALSE)</f>
-        <v>SDG: SG_NHR_NOAPPLN</v>
+        <v>SDG: SE_ADT_ACTS</v>
       </c>
     </row>
     <row r="414" spans="1:11" x14ac:dyDescent="0.35">
@@ -28608,11 +28608,11 @@
         <v>PCNT</v>
       </c>
       <c r="H414" s="1" t="s">
-        <v>4124</v>
+        <v>4240</v>
       </c>
       <c r="I414" s="25" t="str">
         <f>VLOOKUP(H414,Source!$A$2:$G$471,3,FALSE)</f>
-        <v>SDG: IT_USE_ii99</v>
+        <v>SDG: SE_ADT_ACTS</v>
       </c>
     </row>
     <row r="415" spans="1:11" x14ac:dyDescent="0.35">
@@ -28641,7 +28641,7 @@
         <v>PCNT</v>
       </c>
       <c r="H415" s="1" t="s">
-        <v>4125</v>
+        <v>4241</v>
       </c>
       <c r="I415" s="25" t="str">
         <f>VLOOKUP(H415,Source!$A$2:$G$471,3,FALSE)</f>
@@ -28674,7 +28674,7 @@
         <v>PCNT</v>
       </c>
       <c r="H416" s="1" t="s">
-        <v>4239</v>
+        <v>4242</v>
       </c>
       <c r="I416" s="25" t="str">
         <f>VLOOKUP(H416,Source!$A$2:$G$471,3,FALSE)</f>
@@ -28707,7 +28707,7 @@
         <v>PCNT</v>
       </c>
       <c r="H417" s="1" t="s">
-        <v>4240</v>
+        <v>4243</v>
       </c>
       <c r="I417" s="25" t="str">
         <f>VLOOKUP(H417,Source!$A$2:$G$471,3,FALSE)</f>
@@ -28740,7 +28740,7 @@
         <v>PCNT</v>
       </c>
       <c r="H418" s="1" t="s">
-        <v>4241</v>
+        <v>4244</v>
       </c>
       <c r="I418" s="25" t="str">
         <f>VLOOKUP(H418,Source!$A$2:$G$471,3,FALSE)</f>
@@ -28773,7 +28773,7 @@
         <v>PCNT</v>
       </c>
       <c r="H419" s="1" t="s">
-        <v>4242</v>
+        <v>4245</v>
       </c>
       <c r="I419" s="25" t="str">
         <f>VLOOKUP(H419,Source!$A$2:$G$471,3,FALSE)</f>
@@ -28806,7 +28806,7 @@
         <v>PCNT</v>
       </c>
       <c r="H420" s="1" t="s">
-        <v>4243</v>
+        <v>4246</v>
       </c>
       <c r="I420" s="25" t="str">
         <f>VLOOKUP(H420,Source!$A$2:$G$471,3,FALSE)</f>
@@ -28839,11 +28839,11 @@
         <v>PCNT</v>
       </c>
       <c r="H421" s="1" t="s">
-        <v>4244</v>
+        <v>4247</v>
       </c>
       <c r="I421" s="25" t="str">
         <f>VLOOKUP(H421,Source!$A$2:$G$471,3,FALSE)</f>
-        <v>SDG: SE_ADT_ACTS</v>
+        <v>SDG: IT_MOB_OWN</v>
       </c>
     </row>
     <row r="422" spans="1:9" x14ac:dyDescent="0.35">
@@ -28872,11 +28872,11 @@
         <v>PCNT</v>
       </c>
       <c r="H422" s="1" t="s">
-        <v>4245</v>
+        <v>4248</v>
       </c>
       <c r="I422" s="25" t="str">
         <f>VLOOKUP(H422,Source!$A$2:$G$471,3,FALSE)</f>
-        <v>SDG: SE_ADT_ACTS</v>
+        <v>OECD: PP_ADOL_TVGM</v>
       </c>
     </row>
     <row r="423" spans="1:9" x14ac:dyDescent="0.35">
@@ -28905,11 +28905,11 @@
         <v>PCNT</v>
       </c>
       <c r="H423" s="1" t="s">
-        <v>4246</v>
+        <v>4249</v>
       </c>
       <c r="I423" s="25" t="str">
         <f>VLOOKUP(H423,Source!$A$2:$G$471,3,FALSE)</f>
-        <v>SDG: SE_ADT_ACTS</v>
+        <v>OECD: PP_ADOL_INET</v>
       </c>
     </row>
     <row r="424" spans="1:9" x14ac:dyDescent="0.35">
@@ -28938,11 +28938,11 @@
         <v>PCNT</v>
       </c>
       <c r="H424" s="1" t="s">
-        <v>4247</v>
+        <v>4250</v>
       </c>
       <c r="I424" s="25" t="str">
         <f>VLOOKUP(H424,Source!$A$2:$G$471,3,FALSE)</f>
-        <v>SDG: IT_MOB_OWN</v>
+        <v>OECD: PP_ADOL_ITXT</v>
       </c>
     </row>
     <row r="425" spans="1:9" x14ac:dyDescent="0.35">
@@ -28971,11 +28971,11 @@
         <v>PCNT</v>
       </c>
       <c r="H425" s="1" t="s">
-        <v>4248</v>
+        <v>4251</v>
       </c>
       <c r="I425" s="25" t="str">
         <f>VLOOKUP(H425,Source!$A$2:$G$471,3,FALSE)</f>
-        <v>OECD: PP_ADOL_TVGM</v>
+        <v>OECD: PP_ADOL_WORK_PAID</v>
       </c>
     </row>
     <row r="426" spans="1:9" x14ac:dyDescent="0.35">
@@ -29004,11 +29004,11 @@
         <v>PCNT</v>
       </c>
       <c r="H426" s="1" t="s">
-        <v>4249</v>
+        <v>4252</v>
       </c>
       <c r="I426" s="25" t="str">
         <f>VLOOKUP(H426,Source!$A$2:$G$471,3,FALSE)</f>
-        <v>OECD: PP_ADOL_INET</v>
+        <v>OECD: PP_ADOL_WORK_HOME</v>
       </c>
     </row>
     <row r="427" spans="1:9" x14ac:dyDescent="0.35">
@@ -29042,11 +29042,11 @@
         <v>PCNT</v>
       </c>
       <c r="H428" s="1" t="s">
-        <v>4250</v>
+        <v>4253</v>
       </c>
       <c r="I428" s="25" t="str">
         <f>VLOOKUP(H428,Source!$A$2:$G$441,3,FALSE)</f>
-        <v>OECD: PP_ADOL_ITXT</v>
+        <v>Helix: ECD_CHLD_U5_LFT-ALN</v>
       </c>
     </row>
     <row r="429" spans="1:9" x14ac:dyDescent="0.35">
@@ -29075,11 +29075,11 @@
         <v>BINARY</v>
       </c>
       <c r="H429" s="1" t="s">
-        <v>4251</v>
+        <v>4254</v>
       </c>
       <c r="I429" s="25" t="str">
         <f>VLOOKUP(H429,Source!$A$2:$G$441,3,FALSE)</f>
-        <v>OECD: PP_ADOL_WORK_PAID</v>
+        <v>Helix: GN_MTNTY_LV_BNFTS</v>
       </c>
     </row>
     <row r="430" spans="1:9" x14ac:dyDescent="0.35">
@@ -29108,11 +29108,11 @@
         <v>BINARY</v>
       </c>
       <c r="H430" s="1" t="s">
-        <v>4252</v>
+        <v>4525</v>
       </c>
       <c r="I430" s="25" t="str">
         <f>VLOOKUP(H430,Source!$A$2:$G$441,3,FALSE)</f>
-        <v>OECD: PP_ADOL_WORK_HOME</v>
+        <v>Helix: GN_PTNTY_LV_BNFTS</v>
       </c>
     </row>
   </sheetData>
@@ -29652,7 +29652,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:M877"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A232" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D240" sqref="D240"/>
     </sheetView>
@@ -44333,7 +44333,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:L107"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
+    <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="I34" sqref="I34"/>
     </sheetView>
   </sheetViews>
@@ -45720,8 +45720,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:K438"/>
   <sheetViews>
-    <sheetView topLeftCell="A205" workbookViewId="0">
-      <selection activeCell="D216" sqref="D216"/>
+    <sheetView topLeftCell="A427" workbookViewId="0">
+      <selection activeCell="C412" sqref="C412"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
unit revision by nahid
</commit_message>
<xml_diff>
--- a/tmee/data_in/data_dictionary/indicator_dictionary_TM_v8.xlsx
+++ b/tmee/data_in/data_dictionary/indicator_dictionary_TM_v8.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/16f1c7c3db740efb/UNICEF/TransMonEE/data-etl/tmee/data_in/data_dictionary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="195" documentId="13_ncr:1_{86B4128F-EE39-4FFF-A907-770A6E4095C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D5B11B69-D058-422D-92D9-4E5B67173C61}"/>
+  <xr:revisionPtr revIDLastSave="199" documentId="13_ncr:1_{86B4128F-EE39-4FFF-A907-770A6E4095C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2C9CAC17-7079-468B-AAEA-C90BF8EC97C8}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Snapshot" sheetId="1" r:id="rId1"/>
@@ -19272,8 +19272,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L560"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
+      <selection activeCell="F53" sqref="F53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -20988,11 +20988,11 @@
         <v>2020</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>556</v>
+        <v>18</v>
       </c>
       <c r="G50" s="1" t="str">
         <f>VLOOKUP(F50,Value_type!$A$2:$I$107,3,FALSE)</f>
-        <v>GDP_PERC</v>
+        <v>PCNT</v>
       </c>
       <c r="H50" s="1" t="s">
         <v>208</v>
@@ -21022,11 +21022,11 @@
         <v>2021</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>556</v>
+        <v>18</v>
       </c>
       <c r="G51" s="1" t="str">
         <f>VLOOKUP(F51,Value_type!$A$2:$I$107,3,FALSE)</f>
-        <v>GDP_PERC</v>
+        <v>PCNT</v>
       </c>
       <c r="H51" s="1" t="s">
         <v>211</v>
@@ -21056,11 +21056,11 @@
         <v>2021</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>557</v>
+        <v>18</v>
       </c>
       <c r="G52" s="1" t="str">
         <f>VLOOKUP(F52,Value_type!$A$2:$I$107,3,FALSE)</f>
-        <v>GOV_EXP_T</v>
+        <v>PCNT</v>
       </c>
       <c r="H52" s="1" t="s">
         <v>214</v>
@@ -21090,11 +21090,11 @@
         <v>2021</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>570</v>
+        <v>18</v>
       </c>
       <c r="G53" s="1" t="str">
         <f>VLOOKUP(F53,Value_type!$A$2:$I$107,3,FALSE)</f>
-        <v>GOV_EXP_HT</v>
+        <v>PCNT</v>
       </c>
       <c r="H53" s="1" t="s">
         <v>217</v>
@@ -21192,11 +21192,11 @@
         <v>2021</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>570</v>
+        <v>18</v>
       </c>
       <c r="G56" s="1" t="str">
         <f>VLOOKUP(F56,Value_type!$A$2:$I$107,3,FALSE)</f>
-        <v>GOV_EXP_HT</v>
+        <v>PCNT</v>
       </c>
       <c r="H56" s="1" t="s">
         <v>226</v>
@@ -21362,11 +21362,11 @@
         <v>2020</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>570</v>
+        <v>18</v>
       </c>
       <c r="G61" s="1" t="str">
         <f>VLOOKUP(F61,Value_type!$A$2:$I$107,3,FALSE)</f>
-        <v>GOV_EXP_HT</v>
+        <v>PCNT</v>
       </c>
       <c r="H61" s="1" t="s">
         <v>241</v>
@@ -27244,11 +27244,11 @@
         <v>2020</v>
       </c>
       <c r="F234" s="1" t="s">
-        <v>556</v>
+        <v>18</v>
       </c>
       <c r="G234" s="1" t="str">
         <f>VLOOKUP(F234,Value_type!$A$2:$I$107,3,FALSE)</f>
-        <v>GDP_PERC</v>
+        <v>PCNT</v>
       </c>
       <c r="H234" s="1" t="s">
         <v>2726</v>
@@ -27278,11 +27278,11 @@
         <v>2020</v>
       </c>
       <c r="F235" s="1" t="s">
-        <v>557</v>
+        <v>18</v>
       </c>
       <c r="G235" s="1" t="str">
         <f>VLOOKUP(F235,Value_type!$A$2:$I$107,3,FALSE)</f>
-        <v>GOV_EXP_T</v>
+        <v>PCNT</v>
       </c>
       <c r="H235" s="1" t="s">
         <v>2727</v>
@@ -27346,11 +27346,11 @@
         <v>2020</v>
       </c>
       <c r="F237" s="1" t="s">
-        <v>559</v>
+        <v>18</v>
       </c>
       <c r="G237" s="1" t="str">
         <f>VLOOKUP(F237,Value_type!$A$2:$I$107,3,FALSE)</f>
-        <v>GOV_EXP_EDU</v>
+        <v>PCNT</v>
       </c>
       <c r="H237" s="1" t="s">
         <v>2729</v>
@@ -27380,11 +27380,11 @@
         <v>2020</v>
       </c>
       <c r="F238" s="1" t="s">
-        <v>559</v>
+        <v>18</v>
       </c>
       <c r="G238" s="1" t="str">
         <f>VLOOKUP(F238,Value_type!$A$2:$I$107,3,FALSE)</f>
-        <v>GOV_EXP_EDU</v>
+        <v>PCNT</v>
       </c>
       <c r="H238" s="1" t="s">
         <v>2730</v>
@@ -27414,11 +27414,11 @@
         <v>2020</v>
       </c>
       <c r="F239" s="1" t="s">
-        <v>559</v>
+        <v>18</v>
       </c>
       <c r="G239" s="1" t="str">
         <f>VLOOKUP(F239,Value_type!$A$2:$I$107,3,FALSE)</f>
-        <v>GOV_EXP_EDU</v>
+        <v>PCNT</v>
       </c>
       <c r="H239" s="1" t="s">
         <v>2731</v>
@@ -27448,11 +27448,11 @@
         <v>2020</v>
       </c>
       <c r="F240" s="1" t="s">
-        <v>559</v>
+        <v>18</v>
       </c>
       <c r="G240" s="1" t="str">
         <f>VLOOKUP(F240,Value_type!$A$2:$I$107,3,FALSE)</f>
-        <v>GOV_EXP_EDU</v>
+        <v>PCNT</v>
       </c>
       <c r="H240" s="1" t="s">
         <v>2732</v>
@@ -27482,11 +27482,11 @@
         <v>2020</v>
       </c>
       <c r="F241" s="1" t="s">
-        <v>559</v>
+        <v>18</v>
       </c>
       <c r="G241" s="1" t="str">
         <f>VLOOKUP(F241,Value_type!$A$2:$I$107,3,FALSE)</f>
-        <v>GOV_EXP_EDU</v>
+        <v>PCNT</v>
       </c>
       <c r="H241" s="1" t="s">
         <v>2797</v>
@@ -27516,11 +27516,11 @@
         <v>2020</v>
       </c>
       <c r="F242" s="1" t="s">
-        <v>559</v>
+        <v>18</v>
       </c>
       <c r="G242" s="1" t="str">
         <f>VLOOKUP(F242,Value_type!$A$2:$I$107,3,FALSE)</f>
-        <v>GOV_EXP_EDU</v>
+        <v>PCNT</v>
       </c>
       <c r="H242" s="1" t="s">
         <v>2798</v>
@@ -31902,11 +31902,11 @@
         <v>2021</v>
       </c>
       <c r="F371" s="1" t="s">
-        <v>556</v>
+        <v>18</v>
       </c>
       <c r="G371" s="1" t="str">
         <f>VLOOKUP(F371,Value_type!$A$2:$I$107,3,FALSE)</f>
-        <v>GDP_PERC</v>
+        <v>PCNT</v>
       </c>
       <c r="H371" s="1" t="s">
         <v>3751</v>
@@ -33373,11 +33373,11 @@
         <v>2021</v>
       </c>
       <c r="F413" s="1" t="s">
-        <v>556</v>
+        <v>18</v>
       </c>
       <c r="G413" s="1" t="str">
         <f>VLOOKUP(F413,Value_type!$A$2:$I$107,3,FALSE)</f>
-        <v>GDP_PERC</v>
+        <v>PCNT</v>
       </c>
       <c r="H413" s="1" t="s">
         <v>4114</v>
@@ -33407,11 +33407,11 @@
         <v>2021</v>
       </c>
       <c r="F414" s="1" t="s">
-        <v>556</v>
+        <v>18</v>
       </c>
       <c r="G414" s="1" t="str">
         <f>VLOOKUP(F414,Value_type!$A$2:$I$107,3,FALSE)</f>
-        <v>GDP_PERC</v>
+        <v>PCNT</v>
       </c>
       <c r="H414" s="1" t="s">
         <v>4115</v>
@@ -33441,11 +33441,11 @@
         <v>2021</v>
       </c>
       <c r="F415" s="1" t="s">
-        <v>556</v>
+        <v>18</v>
       </c>
       <c r="G415" s="1" t="str">
         <f>VLOOKUP(F415,Value_type!$A$2:$I$107,3,FALSE)</f>
-        <v>GDP_PERC</v>
+        <v>PCNT</v>
       </c>
       <c r="H415" s="1" t="s">
         <v>4116</v>
@@ -33475,11 +33475,11 @@
         <v>2021</v>
       </c>
       <c r="F416" s="1" t="s">
-        <v>556</v>
+        <v>18</v>
       </c>
       <c r="G416" s="1" t="str">
         <f>VLOOKUP(F416,Value_type!$A$2:$I$107,3,FALSE)</f>
-        <v>GDP_PERC</v>
+        <v>PCNT</v>
       </c>
       <c r="H416" s="1" t="s">
         <v>4117</v>
@@ -33509,11 +33509,11 @@
         <v>2021</v>
       </c>
       <c r="F417" s="1" t="s">
-        <v>556</v>
+        <v>18</v>
       </c>
       <c r="G417" s="1" t="str">
         <f>VLOOKUP(F417,Value_type!$A$2:$I$107,3,FALSE)</f>
-        <v>GDP_PERC</v>
+        <v>PCNT</v>
       </c>
       <c r="H417" s="1" t="s">
         <v>4118</v>
@@ -33543,11 +33543,11 @@
         <v>2021</v>
       </c>
       <c r="F418" s="1" t="s">
-        <v>556</v>
+        <v>18</v>
       </c>
       <c r="G418" s="1" t="str">
         <f>VLOOKUP(F418,Value_type!$A$2:$I$107,3,FALSE)</f>
-        <v>GDP_PERC</v>
+        <v>PCNT</v>
       </c>
       <c r="H418" s="1" t="s">
         <v>4119</v>
@@ -33577,11 +33577,11 @@
         <v>2021</v>
       </c>
       <c r="F419" s="1" t="s">
-        <v>556</v>
+        <v>18</v>
       </c>
       <c r="G419" s="1" t="str">
         <f>VLOOKUP(F419,Value_type!$A$2:$I$107,3,FALSE)</f>
-        <v>GDP_PERC</v>
+        <v>PCNT</v>
       </c>
       <c r="H419" s="1" t="s">
         <v>4120</v>
@@ -33611,11 +33611,11 @@
         <v>2021</v>
       </c>
       <c r="F420" s="1" t="s">
-        <v>556</v>
+        <v>18</v>
       </c>
       <c r="G420" s="1" t="str">
         <f>VLOOKUP(F420,Value_type!$A$2:$I$107,3,FALSE)</f>
-        <v>GDP_PERC</v>
+        <v>PCNT</v>
       </c>
       <c r="H420" s="1" t="s">
         <v>4121</v>
@@ -33645,11 +33645,11 @@
         <v>2021</v>
       </c>
       <c r="F421" s="1" t="s">
-        <v>557</v>
+        <v>18</v>
       </c>
       <c r="G421" s="1" t="str">
         <f>VLOOKUP(F421,Value_type!$A$2:$I$107,3,FALSE)</f>
-        <v>GOV_EXP_T</v>
+        <v>PCNT</v>
       </c>
       <c r="H421" s="1" t="s">
         <v>4122</v>
@@ -33781,11 +33781,11 @@
         <v>2021</v>
       </c>
       <c r="F425" s="1" t="s">
-        <v>556</v>
+        <v>18</v>
       </c>
       <c r="G425" s="1" t="str">
         <f>VLOOKUP(F425,Value_type!$A$2:$I$107,3,FALSE)</f>
-        <v>GDP_PERC</v>
+        <v>PCNT</v>
       </c>
       <c r="H425" s="1" t="s">
         <v>4126</v>
@@ -35889,11 +35889,11 @@
         <v>2021</v>
       </c>
       <c r="F487" s="1" t="s">
-        <v>556</v>
+        <v>18</v>
       </c>
       <c r="G487" s="1" t="str">
         <f>VLOOKUP(F487,Value_type!$A$2:$I$107,3,FALSE)</f>
-        <v>GDP_PERC</v>
+        <v>PCNT</v>
       </c>
       <c r="H487" s="1" t="s">
         <v>4578</v>
@@ -35923,11 +35923,11 @@
         <v>2021</v>
       </c>
       <c r="F488" s="1" t="s">
-        <v>557</v>
+        <v>18</v>
       </c>
       <c r="G488" s="1" t="str">
         <f>VLOOKUP(F488,Value_type!$A$2:$I$107,3,FALSE)</f>
-        <v>GOV_EXP_T</v>
+        <v>PCNT</v>
       </c>
       <c r="H488" s="1" t="s">
         <v>4579</v>
@@ -35957,11 +35957,11 @@
         <v>2021</v>
       </c>
       <c r="F489" s="1" t="s">
-        <v>556</v>
+        <v>18</v>
       </c>
       <c r="G489" s="1" t="str">
         <f>VLOOKUP(F489,Value_type!$A$2:$I$107,3,FALSE)</f>
-        <v>GDP_PERC</v>
+        <v>PCNT</v>
       </c>
       <c r="H489" s="1" t="s">
         <v>4580</v>
@@ -35991,11 +35991,11 @@
         <v>2021</v>
       </c>
       <c r="F490" s="1" t="s">
-        <v>557</v>
+        <v>18</v>
       </c>
       <c r="G490" s="1" t="str">
         <f>VLOOKUP(F490,Value_type!$A$2:$I$107,3,FALSE)</f>
-        <v>GOV_EXP_T</v>
+        <v>PCNT</v>
       </c>
       <c r="H490" s="1" t="s">
         <v>4581</v>
@@ -38851,9 +38851,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:M1145"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A410" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E427" sqref="E427"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A464" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E474" sqref="E474"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -60922,8 +60922,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:L107"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>